<commit_message>
folterung(enhancement): Add dropdown selections
</commit_message>
<xml_diff>
--- a/cg/data.xlsx
+++ b/cg/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/era882/Desktop/cg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/era882/Desktop/github/cgapp/cg/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>What is your name?</t>
   </si>
@@ -377,7 +377,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +448,9 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
       <c r="E4">
         <v>0</v>
       </c>

</xml_diff>